<commit_message>
new changes / fixing v2 / v.89
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -401,32 +401,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>WC47 NACP</t>
+          <t>Bloque</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Fallo en elevador</t>
+          <t>Incidencia</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2024-05-29</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>12:18:14</t>
+          <t>Hora</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Mañana</t>
+          <t>Turno</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Hora de Reparación</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Tiempo de Reparación</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>MTBF</t>
         </is>
       </c>
     </row>
@@ -553,6 +563,468 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>0.34 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>12:28:57</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12:28:58</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tornillo atascado en tolva</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>12:29:15</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12:29:17</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>12:29:27</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12:29:29</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.31 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12:29:45</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12:29:47</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.25 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Robot no coge busbar</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12:30:06</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>12:30:08</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.27 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>12:30:10</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>12:30:12</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.29 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12:37:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>12:37:03</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>12:37:02</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12:37:04</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12:37:21</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>12:37:23</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.04 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>12:37:23</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>12:37:25</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.17 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>12:37:35</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>12:37:38</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.13 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing theme management / v.90
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1028,6 +1028,636 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>12:42:27</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>12:42:29</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>12:42:32</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>12:42:34</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>12:45:18</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>12:45:19</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>12:45:25</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>12:45:27</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Fallo cámara QR</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>12:45:29</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>12:45:36</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.13 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Fallo cámara QR</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>12:45:31</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>12:45:32</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.10 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>12:55:16</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>12:55:21</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>12:55:29</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>12:55:31</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>12:55:35</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>12:55:37</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0.21 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>12:56:52</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>12:56:54</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>12:56:55</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>12:56:57</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>12:57:43</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>12:57:51</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0:00:08</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>12:57:47</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>12:57:52</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>12:57:50</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>12:57:52</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0.06 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AOI no detecta pieza</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>12:57:54</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>12:57:56</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0.06 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing some excel mods / v.90
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1658,6 +1658,174 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>12:59:56</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>12:59:58</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>12:59:59</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>13:00:01</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>13:00:09</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>13:00:12</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>0.06 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>13:03:37</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>13:03:39</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new methods and fixing some incidences / v.2.0
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1826,6 +1826,440 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>16:40:03</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>16:40:07</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>16:41:16</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>16:41:20</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>16:47:05</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>16:47:27</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>0:00:22</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>16:47:09</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>16:47:28</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>0:00:19</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Fallo fijador tapa</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>16:47:19</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>16:47:32</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>0:00:13</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>0.07 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>16:47:24</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>16:47:30</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>0.11 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>17:02:51</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>17:02:54</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>17:02:56</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>17:03:00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>17:57:13</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>18:00:16</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Noche</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>18:21:34</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Noche</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
email bug fixed / v.2.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2252,9 +2252,73 @@
           <t>Noche</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>18:39:20</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Noche</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>18:43:02</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Noche</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
new interface update and methods for a better app / v.2.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2316,9 +2316,691 @@
           <t>Noche</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>11:27:23</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>11:27:28</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>11:27:39</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>11:27:41</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>0.12 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>11:31:03</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>11:31:06</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>0.19 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>11:31:05</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>11:31:07</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>1.26 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>11:31:11</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>11:31:14</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>0.95 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Power CP</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>11:31:12</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>11:31:14</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>0.78 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>12:09:27</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>12:09:33</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>12:09:32</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>12:09:34</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>12:09:37</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>12:09:38</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>12:14:01</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>12:14:03</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>12:14:14</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>12:14:19</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>1.52 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>No coloca bien el core</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>12:23:32</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>12:23:38</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Fallo visión core</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>12:23:37</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>12:23:39</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Fallo dispensación glue</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>12:30:52</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>12:30:54</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>12:30:55</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>0.03 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2024-05-31</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>12:48:55</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>12:48:57</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>

<commit_message>
fixing new methods and plots / graphs / v.2.8.0
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3006,6 +3006,1896 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>09:12:00</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>09:12:01</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>09:12:03</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>09:12:04</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>09:12:08</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>09:12:11</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0.04 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>09:12:10</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>09:12:11</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>0.06 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>09:28:33</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>09:28:35</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>09:28:39</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>09:28:41</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>09:28:44</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>09:28:45</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>09:30:20</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>09:30:21</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>09:30:22</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>09:30:23</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0.59 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>09:31:07</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>09:31:10</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0.46 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>09:31:14</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>09:31:16</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0.51 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>09:34:41</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>09:34:43</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0.45 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>09:45:19</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>09:45:21</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>09:45:28</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>09:45:30</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>09:54:19</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>09:54:20</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>09:54:27</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>09:54:28</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>09:54:33</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>09:54:34</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0.13 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>10:02:01</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>10:02:02</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>10:02:05</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>10:02:06</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>10:34:45</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>10:34:46</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>10:34:52</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>10:34:53</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>10:36:16</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>10:36:18</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0.12 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Secuencia atornillador</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>10:41:37</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>10:41:38</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>10:41:51</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>10:41:52</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>10:42:29</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>10:42:31</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>0.24 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>NOK Soldad. Plástico+Metal</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>10:47:33</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>10:47:34</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>10:56:52</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>10:56:55</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>10:57:55</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>10:57:56</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>11:03:45</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>11:03:46</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>11:11:55</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>11:11:56</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>11:13:18</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>11:13:19</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>11:13:27</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>11:13:28</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>1.40 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>11:13:29</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>11:13:30</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>0.77 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>11:16:58</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>11:16:59</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>11:18:49</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>11:18:53</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>11:23:47</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>11:23:48</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>11:24:10</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>11:24:11</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>11:28:50</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>11:28:51</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>11:29:36</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>11:29:37</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>No atornilla clips</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>11:29:46</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>11:29:47</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>0.76 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>11:31:30</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>11:31:32</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>0.47 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>11:39:25</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>11:39:27</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>11:52:36</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>11:52:37</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>11:52:41</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>11:52:42</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Sensor de PCB detecta que hay placa cuando no la hay</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>11:52:48</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>11:52:49</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing new graph window / v.3.0
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4896,6 +4896,300 @@
         </is>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>12:23:04</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>12:23:06</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>12:23:11</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>12:23:13</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>12:23:16</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>12:23:17</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>0.12 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>12:39:40</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>12:39:42</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>12:39:49</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>12:39:50</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>12:39:51</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>12:39:52</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>0.14 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>12:39:53</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>12:39:54</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
graphs fixed / updated / v.3.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5190,6 +5190,258 @@
         </is>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>12:51:20</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>12:51:22</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Top cover</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>12:51:30</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>12:51:33</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Cámara no detecta Pcb</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>12:51:32</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>12:51:33</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>0.16 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>12:51:35</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>12:51:36</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>0.10 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>12:52:15</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>12:52:16</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>0.08 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Cámara no detecta busbar</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>12:57:14</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>12:57:15</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>0.23 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bug fixed / v.4.0
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5442,6 +5442,174 @@
         </is>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>09:12:54</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>09:12:56</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>09:13:23</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>09:13:25</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>09:13:28</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>09:13:29</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>0.49 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>09:16:44</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>09:16:44</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some issues fixed and bugs / v.4.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5610,6 +5610,510 @@
         </is>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>09:18:31</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>09:18:32</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>09:19:05</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>09:19:06</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>09:19:18</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>09:19:19</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>0.57 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>09:19:57</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>09:19:57</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>0.39 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>09:20:17</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>09:20:18</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>0.48 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>09:21:12</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>09:21:13</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>09:26:54</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>09:26:55</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>09:26:56</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>09:26:57</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>5.70 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>09:36:19</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>09:36:21</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>2.87 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>09:36:23</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>09:36:24</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>5.04 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>09:36:25</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>09:36:27</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>3.80 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>09:52:34</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>09:52:35</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating errors / fixing issues / v.5.5
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6366,6 +6366,174 @@
         </is>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>09:46:28</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>09:46:29</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>09:46:41</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>09:46:42</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>09:46:44</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>09:46:45</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>09:46:48</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>09:46:50</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix MTBF calculation and display format
- Adjusted MTBF calculation to display in a more user-friendly format (hours and minutes).
- Updated the update_mtbf_display method to reflect changes in MTBF format.
- Modified log_incidence_to_excel to register MTBF values in the new format.
- Ensured MTBF values are calculated and updated correctly when incidents are confirmed.

This commit resolves the issue of MTBF values being displayed in an unintuitive format and ensures accurate logging of MTBF data.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6534,6 +6534,426 @@
         </is>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>09:53:28</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>09:53:29</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foams</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>09:53:30</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>09:53:31</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Cámara no detecta foam derecho</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>09:53:38</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>09:53:38</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>09:57:07</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>09:57:08</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Ascensor no sube</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>09:57:10</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>09:57:12</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>09:57:13</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>09:57:15</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>0.02 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>09:57:30</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>09:57:31</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>0.05 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>09:58:21</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>09:59:09</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>0:00:48</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>0.12 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>09:59:30</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>09:59:36</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>0:00:06</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>0.20 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>09:59:49</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>09:59:51</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>0.19 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix and improve session-specific incident display and change history
- Update `update_top_incidents` to filter incidents by the current user's blocks.
- Fix `update_change_history` to load and display change history correctly.
- Ensure `log_change` correctly logs changes to the change log file.
- Call `update_change_history` and `update_top_incidents` during UI initialization.

These changes ensure that only session-specific incidents are displayed and the change history is properly shown in the application.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H158"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6954,6 +6954,300 @@
         </is>
       </c>
     </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>10:35:35</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>10:35:36</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Robot no coge PCB</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>10:35:38</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>10:35:40</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>10:36:59</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>10:37:00</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>0.23 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>10:48:07</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>10:48:09</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>10:48:10</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>10:48:12</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>10:48:43</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>10:48:46</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>0.10 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Error en sensor de salida</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>10:48:51</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>10:48:52</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>0.09 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix and improve real-time update of change history
- Update `update_top_incidents` to filter incidents by the current user's blocks.
- Ensure `log_change` correctly logs changes to the change log file.
- Call `update_change_history` after logging each change to update the UI in real-time.
- Ensure relevant changes are logged and displayed immediately in the change history.

These changes ensure that only session-specific incidents are displayed, and the change history is updated in real-time to reflect all changes made in the application.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H165"/>
+  <dimension ref="A1:H170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7248,6 +7248,216 @@
         </is>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>10:56:38</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>10:56:40</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Fallo cámara cover</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>10:56:51</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>10:56:56</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>0.05 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>10:57:07</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>10:57:11</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>0.08 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>10:58:13</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>10:58:18</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>0:00:05</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>0.20 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>10:58:32</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>10:58:33</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>0.19 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix and ensure single instance of general chart
- Ensure the chart display area is properly cleared before drawing a new chart.
- Close any previous figure to avoid displaying old charts.
- Implement horizontal bar chart for better readability of incident labels.
- Modify incident labels to exclude block names, relying on the legend for block identification.
- Ensure `show_general_chart` correctly updates and displays the general chart.

These changes ensure that only the latest instance of the general incident chart is displayed, and improve the readability of the chart by simplifying the incident labels.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H170"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7458,6 +7458,216 @@
         </is>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>NOK Soldadura metal</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>11:25:14</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>11:25:15</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>11:25:20</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>11:25:21</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>0.02 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Fallo cámara ferrite</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>11:25:53</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>11:25:57</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>0.11 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>11:32:58</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>11:32:59</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>11:36:34</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>11:36:36</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve general chart visualization in TurnChart
- Implement horizontal bar chart for better readability of incident labels.
- Organize incidents by block and group them by color using a predefined color palette.
- Reposition legend to avoid overlapping with the bars.
- Ensure TurnChart correctly updates and displays the general chart.

These changes ensure that the general incident chart is displayed with improved readability and organization.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7946,11 +7946,135 @@
           <t>Mañana</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr"/>
-      <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr">
         <is>
           <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>No detecta marcas Power</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>12:04:52</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>12:04:53</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>12:08:34</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>12:08:36</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>12:13:59</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>12:14:00</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance General Chart: Resize for better readability, group incidents by color, and adjust legend positioning
- Reduced the size of the general chart for improved readability of all incidents and legend.
- Grouped incidents by block using a defined color palette for clearer visualization.
- Adjusted the positioning and formatting of the legend to avoid overlapping with the chart bars.
- Applied a soft color palette (shades of blue, brown, orange) for better aesthetics.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H196"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8540,6 +8540,552 @@
         </is>
       </c>
     </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>09:18:43</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>09:18:44</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Fallo etiqueta</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>09:18:49</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>09:18:50</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>0.02 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>09:19:06</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>09:19:07</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>0.06 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>09:28:36</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>09:28:38</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>09:29:11</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>09:29:11</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>0.14 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>09:29:14</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>09:29:14</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>0.10 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>09:29:17</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>09:29:17</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>0.08 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>09:34:07</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>09:34:08</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>09:37:55</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>09:37:56</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>NOK Soldadura Plástico</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>09:40:13</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>09:40:16</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Robot no coloca bien filter en palet</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>09:40:15</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>09:40:16</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>09:42:19</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>09:42:20</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>0.35 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>09:42:23</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>09:42:23</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>0.27 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust application window size and position based on screen resolution
- Implemented `center_window_app` method to resize and center the window based on screen resolution.
- Adjusted window size to 80% of screen width and height for better visibility.
- Called `center_window_app` in `initUI` to position the window correctly after setting its size.
- Ensured the application window opens centrally and fits well on different screen resolutions.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H209"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9086,6 +9086,48 @@
         </is>
       </c>
     </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>10:46:54</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>10:46:56</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Persist detailed messages across sessions
- Added methods to save and load detailed messages to/from a JSON file.
- Modified `add_incidence_details` to save messages when added.
- Ensured detailed messages are saved when the application is closed.
- Added timestamp and incidence information to each detailed message.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:H211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9128,6 +9128,48 @@
         </is>
       </c>
     </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>11:06:56</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>11:07:07</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>0:00:11</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve visualization and functionality of detailed messages
- Added styles for selected items in the detailed messages list to improve visibility.
- Updated add_incidence_details to display only the time of message creation.
- Ensured detailed messages are saved and loaded correctly from a JSON file.
- Enhanced the user experience by making detailed messages more readable.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9170,6 +9170,48 @@
         </is>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>11:19:58</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>11:19:59</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add daily reset for detailed messages
- Implement reset_detailed_messages method to clear detailed messages and save to JSON file.
- Modify schedule_daily_reset to include reset_detailed_messages for daily execution.
- Ensure detailed messages are cleared and saved appropriately.
- Improve the visual display and functionality of the detailed messages tab.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H212"/>
+  <dimension ref="A1:H220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9212,6 +9212,332 @@
         </is>
       </c>
     </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>11:27:21</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>11:27:24</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>11:27:37</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>11:27:41</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>0.07 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Busbar</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>11:37:49</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>11:38:06</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>0:00:17</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Screw K30 no lo detecta puesto</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>11:53:14</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>11:55:22</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>11:55:25</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>11:55:34</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>11:55:35</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>0.05 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>12:10:03</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>12:10:05</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>WC49 P5H</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>La cámara no detecta Top Cover</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>12:12:11</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>12:12:12</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing MTBF data is saved and loaded correctly
- Load MTBF data on application startup.
- Save MTBF data when the application is closed.
- Ensure MTBF calculations use the loaded data for accurate updates.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9538,6 +9538,416 @@
         </is>
       </c>
     </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>12:32:40</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>12:32:43</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Fallo atornillador</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>12:32:53</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>12:32:55</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>0.05 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>12:33:15</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>12:33:24</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>0:00:09</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Fallo tornillo</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>12:37:21</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>12:37:23</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>12:37:28</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>12:37:31</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>0.03 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Fallo en elevador</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>12:38:20</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>12:38:22</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>12:38:24</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>12:38:26</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>0.02 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>12:38:59</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>12:40:29</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>12:40:36</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>0:00:07</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>2024-06-11</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>12:40:38</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>12:40:42</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>0:00:04</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>0.04 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Include 'dependencies' module in PyInstaller build
- Ensured 'dependencies' module is present in the project directory.
- Verified 'dependencies' is installed in the Python environment.
- Modified PyInstaller spec file to include 'dependencies' module in the build process.
- Updated import statements for relative imports where necessary.
- Added configuration in 'beta_version.spec' to include 'dependencies' module paths.

This commit ensures that the 'dependencies' module is properly packaged with the application executable, preventing runtime import errors.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H230"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9948,6 +9948,216 @@
         </is>
       </c>
     </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>09:15:03</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>09:15:05</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>09:31:39</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>09:31:40</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Fallo cámara visión</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>09:31:44</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>09:31:45</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>0.02 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>10:37:10</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>10:37:11</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>0:00:01</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>10:37:13</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>10:37:13</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>0:00:00</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct path specification in .spec file to ensure module inclusion
- Updated `beta_version.spec` to use correct path for the main script.
- Ensured all necessary modules are included in the PyInstaller build process with correct paths.

This commit fixes path issues and ensures that the necessary modules are properly packaged with the application executable.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H235"/>
+  <dimension ref="A1:H236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10158,6 +10158,48 @@
         </is>
       </c>
     </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>WC48 P5F</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>AOI (fallo etiqueta)</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>11:07:19</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>11:07:21</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>0:00:02</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve General Incidences Visualization and Generate New Executable
- Edited the General Incidences list for better visualization.
- Improved grouping and color-coding in the general chart.
- Generated a new executable using PyInstaller with updated configurations.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H238"/>
+  <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10284,6 +10284,124 @@
         </is>
       </c>
     </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Fallo en paletizador</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>10:35:54</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>10:36:09</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>0:00:15</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>No pone tornillo</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>10:36:23</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>10:36:26</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>0:00:03</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>0.12 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Cover atascasdo</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>10:53:07</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr"/>
+      <c r="G241" t="inlineStr"/>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix relative import issues and adjust project structure
Resolved ImportError by converting relative imports to absolute imports and ensuring each directory within the 'app' package contains an __init__.py file. Adjusted script execution context to align with the modified project structure to ensure correct module resolution.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H241"/>
+  <dimension ref="A1:H242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10394,11 +10394,43 @@
           <t>Mañana</t>
         </is>
       </c>
-      <c r="F241" t="inlineStr"/>
-      <c r="G241" t="inlineStr"/>
       <c r="H241" t="inlineStr">
         <is>
           <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>12:15:06</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr"/>
+      <c r="G242" t="inlineStr"/>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor incidence tracking system
- Modified the handling of confirmed incidents to store each confirmation as an individual record instead of just counting them.
- Updated relevant methods to support this new data structure.
- Adjusted the global incidence list display to reflect each confirmation event as a separate item.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H242"/>
+  <dimension ref="A1:H244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10426,11 +10426,75 @@
           <t>Mañana</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr"/>
-      <c r="G242" t="inlineStr"/>
       <c r="H242" t="inlineStr">
         <is>
           <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>12:40:07</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Traza</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>12:40:16</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr"/>
+      <c r="G244" t="inlineStr"/>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>0.03 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance Real-Time Updates Across Application
- Implemented the update_all() method to refresh UI elements effectively after any administrative changes.
- Ensured that all components like global incident lists, tabs, and charts reflect the latest data modifications.
- Connected AdminDialog modifications with the main interface to maintain data consistency across the application.
- Added error handling in update_all() to improve reliability and performance.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H244"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10490,11 +10490,107 @@
           <t>Mañana</t>
         </is>
       </c>
-      <c r="F244" t="inlineStr"/>
-      <c r="G244" t="inlineStr"/>
       <c r="H244" t="inlineStr">
         <is>
           <t>0.03 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>09:59:21</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>09:59:38</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>0.07 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>AAAA</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>09:59:40</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr"/>
+      <c r="G247" t="inlineStr"/>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>0.05 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated beta_version.spec to ensure correct file paths and dependencies
This commit updates the beta_version.spec file to correctly include all necessary dependencies, static files, and hidden imports. Adjustments have been made to ensure that all paths are accurate and relative to the project structure, facilitating the creation of a standalone executable using PyInstaller. This setup ensures that all required resources are packaged with the application, supporting deployment across different environments.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/v2_management.xlsx
+++ b/beta_version/excel_files/v2_management.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H247"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10586,11 +10586,107 @@
           <t>Mañana</t>
         </is>
       </c>
-      <c r="F247" t="inlineStr"/>
-      <c r="G247" t="inlineStr"/>
       <c r="H247" t="inlineStr">
         <is>
           <t>0.05 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Pieza enganchada en HV Test</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>10:01:50</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>-0.00 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>10:01:53</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>0.01 minutos</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Repeat funcional</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>10:02:05</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr"/>
+      <c r="G250" t="inlineStr"/>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>0.04 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>